<commit_message>
fixing bug in bi report
</commit_message>
<xml_diff>
--- a/data/Bioinformation_5_24.xlsx
+++ b/data/Bioinformation_5_24.xlsx
@@ -1522,10 +1522,10 @@
         <v/>
       </c>
       <c r="BP3" s="26" t="n">
-        <v>6.85833333333334</v>
+        <v>6.868750000000006</v>
       </c>
       <c r="BQ3" s="26" t="n">
-        <v>12.01041666666667</v>
+        <v>12</v>
       </c>
       <c r="BR3" s="26" t="n">
         <v/>
@@ -1747,10 +1747,10 @@
         <v/>
       </c>
       <c r="BP4" s="26" t="n">
-        <v>5.989583333333334</v>
+        <v>6</v>
       </c>
       <c r="BQ4" s="26" t="n">
-        <v>14.01041666666667</v>
+        <v>14</v>
       </c>
       <c r="BR4" s="26" t="n">
         <v/>
@@ -1972,10 +1972,10 @@
         <v/>
       </c>
       <c r="BP5" s="26" t="n">
-        <v>13.01666666666667</v>
+        <v>14.3</v>
       </c>
       <c r="BQ5" s="26" t="n">
-        <v>6.010416666666667</v>
+        <v>6</v>
       </c>
       <c r="BR5" s="26" t="n">
         <v/>
@@ -2197,10 +2197,10 @@
         <v/>
       </c>
       <c r="BP6" s="26" t="n">
-        <v>10.95000000000001</v>
+        <v>10.96041666666667</v>
       </c>
       <c r="BQ6" s="26" t="n">
-        <v>11.01041666666667</v>
+        <v>11</v>
       </c>
       <c r="BR6" s="26" t="n">
         <v/>
@@ -2422,10 +2422,10 @@
         <v/>
       </c>
       <c r="BP7" s="26" t="n">
-        <v>18.48125</v>
+        <v>18.49166666666667</v>
       </c>
       <c r="BQ7" s="26" t="n">
-        <v>5.016666666666667</v>
+        <v>5.00625</v>
       </c>
       <c r="BR7" s="26" t="n">
         <v/>

</xml_diff>